<commit_message>
add dataDict and Authorizations
</commit_message>
<xml_diff>
--- a/dataDictionary.xlsx
+++ b/dataDictionary.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyhoffman/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyhoffman/Desktop/DatabaseCourseProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="13860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -260,6 +260,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
@@ -286,9 +287,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -581,26 +582,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
@@ -658,12 +659,12 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
@@ -677,7 +678,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -688,7 +689,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
@@ -699,7 +700,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="s">
@@ -710,7 +711,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B13" t="s">
@@ -721,7 +722,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B14" t="s">
@@ -732,7 +733,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B15" t="s">
@@ -743,12 +744,12 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B17" t="s">
@@ -762,7 +763,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B18" t="s">
@@ -773,7 +774,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B19" t="s">
@@ -784,12 +785,12 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B21" t="s">
@@ -803,7 +804,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B22" t="s">
@@ -814,7 +815,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B23" t="s">
@@ -825,7 +826,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B24" t="s">
@@ -836,12 +837,12 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B26" t="s">
@@ -855,7 +856,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B27" t="s">
@@ -869,7 +870,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B28" t="s">
@@ -883,12 +884,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B30" t="s">
@@ -902,7 +903,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B31" t="s">
@@ -916,7 +917,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B32" t="s">
@@ -927,7 +928,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B33" t="s">
@@ -941,12 +942,12 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B35" t="s">
@@ -957,7 +958,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B36" t="s">

</xml_diff>

<commit_message>
Final Relational model - UPDATED
</commit_message>
<xml_diff>
--- a/dataDictionary.xlsx
+++ b/dataDictionary.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyhoffman/Desktop/DatabaseCourseProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suhas\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
   <si>
     <t>DATA ITEM</t>
   </si>
@@ -56,15 +56,9 @@
     <t>can't be null</t>
   </si>
   <si>
-    <t xml:space="preserve">name </t>
-  </si>
-  <si>
     <t>name of the student</t>
   </si>
   <si>
-    <t>birth date</t>
-  </si>
-  <si>
     <t>date of birth of the student</t>
   </si>
   <si>
@@ -77,9 +71,6 @@
     <t>Location where student lives</t>
   </si>
   <si>
-    <t>gender</t>
-  </si>
-  <si>
     <t>sex of the student</t>
   </si>
   <si>
@@ -206,9 +197,6 @@
     <t xml:space="preserve">The credit card number used to pay </t>
   </si>
   <si>
-    <t>expDate</t>
-  </si>
-  <si>
     <t>the 4 integer expiration date on the card</t>
   </si>
   <si>
@@ -237,12 +225,36 @@
   </si>
   <si>
     <t>nameOnCard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">studentname </t>
+  </si>
+  <si>
+    <t>birthdate</t>
+  </si>
+  <si>
+    <t>studentgender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coursename </t>
+  </si>
+  <si>
+    <t xml:space="preserve">universityname </t>
+  </si>
+  <si>
+    <t xml:space="preserve">instructorname </t>
+  </si>
+  <si>
+    <t>instructorgender</t>
+  </si>
+  <si>
+    <t>expirydate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -299,6 +311,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -569,19 +584,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -595,12 +610,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -608,376 +623,376 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="B27" t="s">
         <v>49</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C27" t="s">
         <v>50</v>
       </c>
-      <c r="C26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>52</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>55</v>
       </c>
-      <c r="C28" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" t="s">
         <v>57</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C30" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="B33" t="s">
         <v>59</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" t="s">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="B35" t="s">
         <v>62</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C33" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="B36" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" t="s">
-        <v>68</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>

</xml_diff>